<commit_message>
Corrected files for porduction.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/Hardware/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_timestamp_generator_Gen3\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\device.timestampgeneratorgen3\Hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79593696-83CE-4F78-91AB-BED3CDCDB72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6BAE8-BC46-4C40-9BDD-895685BF9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="193">
   <si>
     <t>Value</t>
   </si>
@@ -194,9 +194,6 @@
     <t>R33, R34, R35, R36, R37, R40, R41, R42, R44, R45</t>
   </si>
   <si>
-    <t xml:space="preserve">RC0402FR-07330RL </t>
-  </si>
-  <si>
     <t>330nF</t>
   </si>
   <si>
@@ -642,6 +639,15 @@
   </si>
   <si>
     <t>04025A470JAT2A</t>
+  </si>
+  <si>
+    <t>RC0402FR-07330RL</t>
+  </si>
+  <si>
+    <t>Number of SMD unique parts</t>
+  </si>
+  <si>
+    <t>Number of TH unique parts</t>
   </si>
 </sst>
 </file>
@@ -1165,6 +1171,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1173,9 +1182,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1532,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F50C34B-C9F6-4E1C-A615-C6E180679338}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1550,7 @@
     <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="35.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -1569,30 +1575,30 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="E3" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>18</v>
@@ -1609,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>19</v>
@@ -1623,16 +1629,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>18</v>
@@ -1643,15 +1649,15 @@
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="12">
+        <v>44</v>
+      </c>
+      <c r="E6" s="9">
         <v>885012205084</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -1663,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>18</v>
@@ -1683,16 +1689,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>18</v>
@@ -1703,16 +1709,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>18</v>
@@ -1723,16 +1729,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>152</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>17</v>
@@ -1743,16 +1749,16 @@
         <v>1</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>18</v>
@@ -1763,16 +1769,16 @@
         <v>7</v>
       </c>
       <c r="B12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="D12" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>18</v>
@@ -1783,7 +1789,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>27</v>
@@ -1792,7 +1798,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>18</v>
@@ -1803,19 +1809,19 @@
         <v>2</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>163</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1823,16 +1829,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>102</v>
-      </c>
       <c r="E15" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>18</v>
@@ -1843,16 +1849,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>18</v>
@@ -1863,22 +1869,22 @@
         <v>6</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1886,16 +1892,16 @@
         <v>1</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>114</v>
-      </c>
       <c r="E18" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>18</v>
@@ -1906,16 +1912,16 @@
         <v>1</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>18</v>
@@ -1926,16 +1932,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>18</v>
@@ -1946,16 +1952,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>18</v>
@@ -1966,16 +1972,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="E22" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>18</v>
@@ -1986,16 +1992,16 @@
         <v>3</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="E23" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>18</v>
@@ -2006,16 +2012,16 @@
         <v>1</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>18</v>
@@ -2026,19 +2032,19 @@
         <v>5</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="E25" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2046,16 +2052,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="E26" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>18</v>
@@ -2066,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>24</v>
@@ -2075,7 +2081,7 @@
         <v>25</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>17</v>
@@ -2086,16 +2092,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="E28" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>18</v>
@@ -2106,16 +2112,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>18</v>
@@ -2126,16 +2132,16 @@
         <v>1</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>18</v>
@@ -2146,16 +2152,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>18</v>
@@ -2166,16 +2172,16 @@
         <v>1</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="E32" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>18</v>
@@ -2195,7 +2201,7 @@
         <v>8</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F33" s="7" t="s">
         <v>18</v>
@@ -2215,7 +2221,7 @@
         <v>28</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F34" s="7" t="s">
         <v>18</v>
@@ -2226,16 +2232,16 @@
         <v>3</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>18</v>
@@ -2246,7 +2252,7 @@
         <v>1</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>37</v>
@@ -2255,7 +2261,7 @@
         <v>38</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>18</v>
@@ -2276,7 +2282,7 @@
         <v>32</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F37" s="7" t="s">
         <v>18</v>
@@ -2287,37 +2293,39 @@
         <v>1</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="F38" s="7"/>
+        <v>185</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>1</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2331,7 +2339,7 @@
         <v>9</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>36</v>
@@ -2351,10 +2359,10 @@
         <v>9</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>18</v>
@@ -2374,7 +2382,7 @@
         <v>40</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>41</v>
+        <v>190</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>18</v>
@@ -2385,16 +2393,16 @@
         <v>1</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>55</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="F43" s="7" t="s">
         <v>18</v>
@@ -2405,13 +2413,13 @@
         <v>2</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>33</v>
@@ -2431,10 +2439,10 @@
         <v>9</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F45" s="7" t="s">
         <v>18</v>
@@ -2445,16 +2453,16 @@
         <v>1</v>
       </c>
       <c r="B46" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="D46" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>17</v>
@@ -2465,16 +2473,16 @@
         <v>10</v>
       </c>
       <c r="B47" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="E47" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="F47" s="7" t="s">
         <v>18</v>
@@ -2485,16 +2493,16 @@
         <v>1</v>
       </c>
       <c r="B48" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>18</v>
@@ -2505,16 +2513,16 @@
         <v>1</v>
       </c>
       <c r="B49" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>160</v>
-      </c>
       <c r="E49" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F49" s="7" t="s">
         <v>17</v>
@@ -2525,30 +2533,30 @@
         <v>1</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D50" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="E50" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
@@ -2557,10 +2565,10 @@
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52" t="s">
+        <v>133</v>
+      </c>
+      <c r="E52" t="s">
         <v>134</v>
-      </c>
-      <c r="E52" t="s">
-        <v>135</v>
       </c>
       <c r="F52" s="4"/>
     </row>
@@ -2571,10 +2579,10 @@
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F53" s="4"/>
     </row>
@@ -2585,10 +2593,10 @@
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" t="s">
         <v>137</v>
-      </c>
-      <c r="E54" t="s">
-        <v>138</v>
       </c>
       <c r="F54" s="4"/>
     </row>
@@ -2599,10 +2607,10 @@
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55" t="s">
+        <v>145</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>15</v>
@@ -2615,22 +2623,22 @@
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56" t="s">
+        <v>138</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>140</v>
-      </c>
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
+      <c r="A57" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
@@ -2639,10 +2647,10 @@
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58" t="s">
+        <v>131</v>
+      </c>
+      <c r="E58" t="s">
         <v>132</v>
-      </c>
-      <c r="E58" t="s">
-        <v>133</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>15</v>
@@ -2655,10 +2663,10 @@
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" t="s">
         <v>141</v>
-      </c>
-      <c r="E59" t="s">
-        <v>142</v>
       </c>
       <c r="F59" s="4"/>
     </row>
@@ -2669,33 +2677,33 @@
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60" t="s">
+        <v>142</v>
+      </c>
+      <c r="E60" t="s">
         <v>143</v>
       </c>
-      <c r="E60" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E62" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F62" s="1">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E63" s="3" t="s">
-        <v>12</v>
+        <v>191</v>
       </c>
       <c r="F63" s="1">
         <v>42</v>
@@ -2703,10 +2711,26 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E65" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F65" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E66" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F64" s="1">
-        <v>4</v>
+      <c r="F66" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced Q5 with a correct size component.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/harp timestamp generator Gen3 BOM.xlsx
+++ b/Hardware/PCB/harp timestamp generator Gen3 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\device.timestampgeneratorgen3\Hardware\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C6BAE8-BC46-4C40-9BDD-895685BF9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73603C72-5FE9-47FE-A052-A893694266C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp timestamp generator" sheetId="13" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="194">
   <si>
     <t>Value</t>
   </si>
@@ -648,6 +648,9 @@
   </si>
   <si>
     <t>Number of TH unique parts</t>
+  </si>
+  <si>
+    <t>PMF170XP,115</t>
   </si>
 </sst>
 </file>
@@ -1540,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F50C34B-C9F6-4E1C-A615-C6E180679338}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,7 +2184,7 @@
         <v>85</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>84</v>
+        <v>193</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>18</v>

</xml_diff>